<commit_message>
Weird Color of excel.
</commit_message>
<xml_diff>
--- a/assets/Dataset_results.xlsx
+++ b/assets/Dataset_results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yimuyuan/Documents/codes/labs/kaggle/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yimuyuan/Documents/codes/labs/kaggle/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D495E2B8-0C8A-C249-BA1C-97A0154ABD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF38B3C6-F0C9-CE47-A732-29D9E878AFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="760" windowWidth="27640" windowHeight="17720" xr2:uid="{D5CB6DED-93DD-3F4C-A27E-ABB2A23A610F}"/>
   </bookViews>
@@ -508,7 +508,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -560,6 +570,59 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -2203,14 +2266,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4783255A-B592-BF42-8F92-917F24389843}">
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:XFD73"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="54.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" customWidth="1"/>
+    <col min="5" max="7" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -3901,27 +3964,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E73">
-    <cfRule type="expression" dxfId="8" priority="4">
-      <formula xml:space="preserve"> E2 &lt; F2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="5">
-      <formula>E2 &gt; F2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="7">
-      <formula>$E$2:$E$73 &gt; $F$2:$F$73</formula>
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>AND(E2&gt;F2, E2&gt;G2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F73">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>F2&gt;G2</formula>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>AND(F2&gt;E2,F2&gt;G2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G73">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>G2&gt;E2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>G2&gt;F2</formula>
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(G2&gt;E2,G2&gt;F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>